<commit_message>
completed migration of text file to excel sheet
</commit_message>
<xml_diff>
--- a/MyCompanyStaff.xlsx
+++ b/MyCompanyStaff.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Employees" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -122,6 +122,21 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table" displayName="Table" ref="A1:G2" headerRowCount="1">
+  <autoFilter ref="A1:G2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="First Name"/>
+    <tableColumn id="3" name="Last Name"/>
+    <tableColumn id="4" name="Department"/>
+    <tableColumn id="5" name="Phone"/>
+    <tableColumn id="6" name="Address"/>
+    <tableColumn id="7" name="Salary"/>
+  </tableColumns>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,19 +423,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Salary</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Luke</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Phillip</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1232123</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1st Address, Miami</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>52000</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>